<commit_message>
updating original regression analysis for paper
</commit_message>
<xml_diff>
--- a/GSD/baskets_new_sizes/quadrant_analysis.xlsx
+++ b/GSD/baskets_new_sizes/quadrant_analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\GSD\baskets_new_sizes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\La_Jara\GSD\baskets_new_sizes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{09856145-D96D-4DB5-95FD-C464AE3E43D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2195E0B9-60FE-4E6E-B11C-0CB6A383E6DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" xr2:uid="{9F4E2E31-D1B5-41CC-A282-6545E5272E61}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9F4E2E31-D1B5-41CC-A282-6545E5272E61}"/>
   </bookViews>
   <sheets>
     <sheet name="Original Sizes" sheetId="1" r:id="rId1"/>
@@ -308,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -376,9 +376,6 @@
     <xf numFmtId="165" fontId="3" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -400,22 +397,16 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3735,27 +3726,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="I2" s="31" t="s">
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="I2" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="O2" s="23" t="s">
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="O2" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
       <c r="V2" s="32" t="s">
         <v>26</v>
       </c>
@@ -3814,13 +3805,13 @@
       <c r="S3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="V3" s="35" t="s">
+      <c r="V3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="W3" s="35" t="s">
+      <c r="W3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="X3" s="35" t="s">
+      <c r="X3" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3834,62 +3825,62 @@
       <c r="C4" s="11">
         <v>-0.41446964008822845</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="23">
         <v>-0.42344355789344579</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="23">
         <v>-0.14476461895714599</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="23">
         <v>-0.17090718766294993</v>
       </c>
-      <c r="G4" s="24">
+      <c r="G4" s="23">
         <v>-0.19519361027032006</v>
       </c>
-      <c r="I4" s="29" t="str">
-        <f>IF(AND($B4&gt;0, C4&gt;0), "Q1", IF(AND($B4&lt;0, C4&gt;0), "Q2", IF(AND($B4&lt;0, C4&lt;0), "Q3", "Q4")))</f>
+      <c r="I4" s="28" t="str">
+        <f t="shared" ref="I4:I14" si="0">IF(AND($B4&gt;0, C4&gt;0), "Q1", IF(AND($B4&lt;0, C4&gt;0), "Q2", IF(AND($B4&lt;0, C4&lt;0), "Q3", "Q4")))</f>
         <v>Q4</v>
       </c>
-      <c r="J4" s="29" t="str">
-        <f>IF(AND($B4&gt;0, D4&gt;0), "Q1", IF(AND($B4&lt;0, D4&gt;0), "Q2", IF(AND($B4&lt;0, D4&lt;0), "Q3", "Q4")))</f>
+      <c r="J4" s="28" t="str">
+        <f t="shared" ref="J4:J14" si="1">IF(AND($B4&gt;0, D4&gt;0), "Q1", IF(AND($B4&lt;0, D4&gt;0), "Q2", IF(AND($B4&lt;0, D4&lt;0), "Q3", "Q4")))</f>
         <v>Q4</v>
       </c>
-      <c r="K4" s="29" t="str">
-        <f>IF(AND($B4&gt;0, E4&gt;0), "Q1", IF(AND($B4&lt;0, E4&gt;0), "Q2", IF(AND($B4&lt;0, E4&lt;0), "Q3", "Q4")))</f>
+      <c r="K4" s="28" t="str">
+        <f t="shared" ref="K4:K14" si="2">IF(AND($B4&gt;0, E4&gt;0), "Q1", IF(AND($B4&lt;0, E4&gt;0), "Q2", IF(AND($B4&lt;0, E4&lt;0), "Q3", "Q4")))</f>
         <v>Q4</v>
       </c>
-      <c r="L4" s="29" t="str">
-        <f>IF(AND($B4&gt;0, F4&gt;0), "Q1", IF(AND($B4&lt;0, F4&gt;0), "Q2", IF(AND($B4&lt;0, F4&lt;0), "Q3", "Q4")))</f>
+      <c r="L4" s="28" t="str">
+        <f t="shared" ref="L4:L14" si="3">IF(AND($B4&gt;0, F4&gt;0), "Q1", IF(AND($B4&lt;0, F4&gt;0), "Q2", IF(AND($B4&lt;0, F4&lt;0), "Q3", "Q4")))</f>
         <v>Q4</v>
       </c>
-      <c r="M4" s="29" t="str">
-        <f>IF(AND($B4&gt;0, G4&gt;0), "Q1", IF(AND($B4&lt;0, G4&gt;0), "Q2", IF(AND($B4&lt;0, G4&lt;0), "Q3", "Q4")))</f>
+      <c r="M4" s="28" t="str">
+        <f t="shared" ref="M4:M14" si="4">IF(AND($B4&gt;0, G4&gt;0), "Q1", IF(AND($B4&lt;0, G4&gt;0), "Q2", IF(AND($B4&lt;0, G4&lt;0), "Q3", "Q4")))</f>
         <v>Q4</v>
       </c>
-      <c r="O4" s="29" t="str">
+      <c r="O4" s="28" t="str">
         <f>IF(OR(I4="Q2", I4="Q4"), "Correct", "Incorrect")</f>
         <v>Correct</v>
       </c>
-      <c r="P4" s="29" t="str">
+      <c r="P4" s="28" t="str">
         <f>IF(OR(J4="Q2", J4="Q4"), "Correct", "Incorrect")</f>
         <v>Correct</v>
       </c>
-      <c r="Q4" s="29" t="str">
+      <c r="Q4" s="28" t="str">
         <f>IF(OR(K4="Q2", K4="Q4"), "Correct", "Incorrect")</f>
         <v>Correct</v>
       </c>
-      <c r="R4" s="29" t="str">
-        <f t="shared" ref="P4:S4" si="0">IF(OR(L4="Q2", L4="Q4"), "Correct", "Incorrect")</f>
-        <v>Correct</v>
-      </c>
-      <c r="S4" s="29" t="str">
-        <f t="shared" si="0"/>
+      <c r="R4" s="28" t="str">
+        <f t="shared" ref="R4:S4" si="5">IF(OR(L4="Q2", L4="Q4"), "Correct", "Incorrect")</f>
+        <v>Correct</v>
+      </c>
+      <c r="S4" s="28" t="str">
+        <f t="shared" si="5"/>
         <v>Correct</v>
       </c>
       <c r="U4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="V4" s="36">
+      <c r="V4" s="11">
         <f>COUNTIF(O$4:O$14, "Correct") / COUNTA(O$4:O$14)</f>
         <v>0.63636363636363635</v>
       </c>
@@ -3924,50 +3915,50 @@
       <c r="G5" s="11">
         <v>-0.66804316680566478</v>
       </c>
-      <c r="I5" s="29" t="str">
-        <f>IF(AND($B5&gt;0, C5&gt;0), "Q1", IF(AND($B5&lt;0, C5&gt;0), "Q2", IF(AND($B5&lt;0, C5&lt;0), "Q3", "Q4")))</f>
+      <c r="I5" s="28" t="str">
+        <f t="shared" si="0"/>
         <v>Q4</v>
       </c>
-      <c r="J5" s="29" t="str">
-        <f>IF(AND($B5&gt;0, D5&gt;0), "Q1", IF(AND($B5&lt;0, D5&gt;0), "Q2", IF(AND($B5&lt;0, D5&lt;0), "Q3", "Q4")))</f>
+      <c r="J5" s="28" t="str">
+        <f t="shared" si="1"/>
         <v>Q4</v>
       </c>
-      <c r="K5" s="29" t="str">
-        <f>IF(AND($B5&gt;0, E5&gt;0), "Q1", IF(AND($B5&lt;0, E5&gt;0), "Q2", IF(AND($B5&lt;0, E5&lt;0), "Q3", "Q4")))</f>
+      <c r="K5" s="28" t="str">
+        <f t="shared" si="2"/>
         <v>Q4</v>
       </c>
-      <c r="L5" s="29" t="str">
-        <f>IF(AND($B5&gt;0, F5&gt;0), "Q1", IF(AND($B5&lt;0, F5&gt;0), "Q2", IF(AND($B5&lt;0, F5&lt;0), "Q3", "Q4")))</f>
+      <c r="L5" s="28" t="str">
+        <f t="shared" si="3"/>
         <v>Q4</v>
       </c>
-      <c r="M5" s="29" t="str">
-        <f>IF(AND($B5&gt;0, G5&gt;0), "Q1", IF(AND($B5&lt;0, G5&gt;0), "Q2", IF(AND($B5&lt;0, G5&lt;0), "Q3", "Q4")))</f>
+      <c r="M5" s="28" t="str">
+        <f t="shared" si="4"/>
         <v>Q4</v>
       </c>
-      <c r="O5" s="29" t="str">
-        <f t="shared" ref="O5:O14" si="1">IF(OR(I5="Q2", I5="Q4"), "Correct", "Incorrect")</f>
-        <v>Correct</v>
-      </c>
-      <c r="P5" s="29" t="str">
-        <f t="shared" ref="P5:P14" si="2">IF(OR(J5="Q2", J5="Q4"), "Correct", "Incorrect")</f>
-        <v>Correct</v>
-      </c>
-      <c r="Q5" s="29" t="str">
-        <f t="shared" ref="Q5:Q14" si="3">IF(OR(K5="Q2", K5="Q4"), "Correct", "Incorrect")</f>
-        <v>Correct</v>
-      </c>
-      <c r="R5" s="29" t="str">
-        <f t="shared" ref="R5:R14" si="4">IF(OR(L5="Q2", L5="Q4"), "Correct", "Incorrect")</f>
-        <v>Correct</v>
-      </c>
-      <c r="S5" s="29" t="str">
-        <f t="shared" ref="S5:S14" si="5">IF(OR(M5="Q2", M5="Q4"), "Correct", "Incorrect")</f>
+      <c r="O5" s="28" t="str">
+        <f t="shared" ref="O5:O14" si="6">IF(OR(I5="Q2", I5="Q4"), "Correct", "Incorrect")</f>
+        <v>Correct</v>
+      </c>
+      <c r="P5" s="28" t="str">
+        <f t="shared" ref="P5:P14" si="7">IF(OR(J5="Q2", J5="Q4"), "Correct", "Incorrect")</f>
+        <v>Correct</v>
+      </c>
+      <c r="Q5" s="28" t="str">
+        <f t="shared" ref="Q5:Q14" si="8">IF(OR(K5="Q2", K5="Q4"), "Correct", "Incorrect")</f>
+        <v>Correct</v>
+      </c>
+      <c r="R5" s="28" t="str">
+        <f t="shared" ref="R5:R14" si="9">IF(OR(L5="Q2", L5="Q4"), "Correct", "Incorrect")</f>
+        <v>Correct</v>
+      </c>
+      <c r="S5" s="28" t="str">
+        <f t="shared" ref="S5:S14" si="10">IF(OR(M5="Q2", M5="Q4"), "Correct", "Incorrect")</f>
         <v>Correct</v>
       </c>
       <c r="U5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="V5" s="36">
+      <c r="V5" s="11">
         <f>COUNTIF(P$4:P$14, "Correct") / COUNTA(P$4:P$14)</f>
         <v>0.72727272727272729</v>
       </c>
@@ -3976,7 +3967,7 @@
         <v>0.27272727272727271</v>
       </c>
       <c r="X5" s="10">
-        <f t="shared" ref="X5:X8" si="6">SUM(V5:W5)</f>
+        <f t="shared" ref="X5:X8" si="11">SUM(V5:W5)</f>
         <v>1</v>
       </c>
     </row>
@@ -4002,50 +3993,50 @@
       <c r="G6" s="11">
         <v>0.49854710443643002</v>
       </c>
-      <c r="I6" s="30" t="str">
-        <f>IF(AND($B6&gt;0, C6&gt;0), "Q1", IF(AND($B6&lt;0, C6&gt;0), "Q2", IF(AND($B6&lt;0, C6&lt;0), "Q3", "Q4")))</f>
+      <c r="I6" s="29" t="str">
+        <f t="shared" si="0"/>
         <v>Q2</v>
       </c>
-      <c r="J6" s="30" t="str">
-        <f>IF(AND($B6&gt;0, D6&gt;0), "Q1", IF(AND($B6&lt;0, D6&gt;0), "Q2", IF(AND($B6&lt;0, D6&lt;0), "Q3", "Q4")))</f>
+      <c r="J6" s="29" t="str">
+        <f t="shared" si="1"/>
         <v>Q2</v>
       </c>
-      <c r="K6" s="30" t="str">
-        <f>IF(AND($B6&gt;0, E6&gt;0), "Q1", IF(AND($B6&lt;0, E6&gt;0), "Q2", IF(AND($B6&lt;0, E6&lt;0), "Q3", "Q4")))</f>
+      <c r="K6" s="29" t="str">
+        <f t="shared" si="2"/>
         <v>Q2</v>
       </c>
-      <c r="L6" s="30" t="str">
-        <f>IF(AND($B6&gt;0, F6&gt;0), "Q1", IF(AND($B6&lt;0, F6&gt;0), "Q2", IF(AND($B6&lt;0, F6&lt;0), "Q3", "Q4")))</f>
+      <c r="L6" s="29" t="str">
+        <f t="shared" si="3"/>
         <v>Q2</v>
       </c>
-      <c r="M6" s="30" t="str">
-        <f>IF(AND($B6&gt;0, G6&gt;0), "Q1", IF(AND($B6&lt;0, G6&gt;0), "Q2", IF(AND($B6&lt;0, G6&lt;0), "Q3", "Q4")))</f>
+      <c r="M6" s="29" t="str">
+        <f t="shared" si="4"/>
         <v>Q2</v>
       </c>
-      <c r="O6" s="29" t="str">
-        <f t="shared" si="1"/>
-        <v>Correct</v>
-      </c>
-      <c r="P6" s="29" t="str">
-        <f t="shared" si="2"/>
-        <v>Correct</v>
-      </c>
-      <c r="Q6" s="29" t="str">
-        <f t="shared" si="3"/>
-        <v>Correct</v>
-      </c>
-      <c r="R6" s="29" t="str">
-        <f t="shared" si="4"/>
-        <v>Correct</v>
-      </c>
-      <c r="S6" s="29" t="str">
-        <f t="shared" si="5"/>
+      <c r="O6" s="28" t="str">
+        <f t="shared" si="6"/>
+        <v>Correct</v>
+      </c>
+      <c r="P6" s="28" t="str">
+        <f t="shared" si="7"/>
+        <v>Correct</v>
+      </c>
+      <c r="Q6" s="28" t="str">
+        <f t="shared" si="8"/>
+        <v>Correct</v>
+      </c>
+      <c r="R6" s="28" t="str">
+        <f t="shared" si="9"/>
+        <v>Correct</v>
+      </c>
+      <c r="S6" s="28" t="str">
+        <f t="shared" si="10"/>
         <v>Correct</v>
       </c>
       <c r="U6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="V6" s="36">
+      <c r="V6" s="11">
         <f>COUNTIF(Q$4:Q$14, "Correct") / COUNTA(Q$4:Q$14)</f>
         <v>0.81818181818181823</v>
       </c>
@@ -4054,7 +4045,7 @@
         <v>0.18181818181818182</v>
       </c>
       <c r="X6" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -4080,50 +4071,50 @@
       <c r="G7" s="11">
         <v>0.9246065038279212</v>
       </c>
-      <c r="I7" s="30" t="str">
-        <f>IF(AND($B7&gt;0, C7&gt;0), "Q1", IF(AND($B7&lt;0, C7&gt;0), "Q2", IF(AND($B7&lt;0, C7&lt;0), "Q3", "Q4")))</f>
+      <c r="I7" s="29" t="str">
+        <f t="shared" si="0"/>
         <v>Q2</v>
       </c>
-      <c r="J7" s="30" t="str">
-        <f>IF(AND($B7&gt;0, D7&gt;0), "Q1", IF(AND($B7&lt;0, D7&gt;0), "Q2", IF(AND($B7&lt;0, D7&lt;0), "Q3", "Q4")))</f>
+      <c r="J7" s="29" t="str">
+        <f t="shared" si="1"/>
         <v>Q2</v>
       </c>
-      <c r="K7" s="30" t="str">
-        <f>IF(AND($B7&gt;0, E7&gt;0), "Q1", IF(AND($B7&lt;0, E7&gt;0), "Q2", IF(AND($B7&lt;0, E7&lt;0), "Q3", "Q4")))</f>
+      <c r="K7" s="29" t="str">
+        <f t="shared" si="2"/>
         <v>Q2</v>
       </c>
-      <c r="L7" s="30" t="str">
-        <f>IF(AND($B7&gt;0, F7&gt;0), "Q1", IF(AND($B7&lt;0, F7&gt;0), "Q2", IF(AND($B7&lt;0, F7&lt;0), "Q3", "Q4")))</f>
+      <c r="L7" s="29" t="str">
+        <f t="shared" si="3"/>
         <v>Q2</v>
       </c>
-      <c r="M7" s="30" t="str">
-        <f>IF(AND($B7&gt;0, G7&gt;0), "Q1", IF(AND($B7&lt;0, G7&gt;0), "Q2", IF(AND($B7&lt;0, G7&lt;0), "Q3", "Q4")))</f>
+      <c r="M7" s="29" t="str">
+        <f t="shared" si="4"/>
         <v>Q2</v>
       </c>
-      <c r="O7" s="29" t="str">
-        <f t="shared" si="1"/>
-        <v>Correct</v>
-      </c>
-      <c r="P7" s="29" t="str">
-        <f t="shared" si="2"/>
-        <v>Correct</v>
-      </c>
-      <c r="Q7" s="29" t="str">
-        <f t="shared" si="3"/>
-        <v>Correct</v>
-      </c>
-      <c r="R7" s="29" t="str">
-        <f t="shared" si="4"/>
-        <v>Correct</v>
-      </c>
-      <c r="S7" s="29" t="str">
-        <f t="shared" si="5"/>
+      <c r="O7" s="28" t="str">
+        <f t="shared" si="6"/>
+        <v>Correct</v>
+      </c>
+      <c r="P7" s="28" t="str">
+        <f t="shared" si="7"/>
+        <v>Correct</v>
+      </c>
+      <c r="Q7" s="28" t="str">
+        <f t="shared" si="8"/>
+        <v>Correct</v>
+      </c>
+      <c r="R7" s="28" t="str">
+        <f t="shared" si="9"/>
+        <v>Correct</v>
+      </c>
+      <c r="S7" s="28" t="str">
+        <f t="shared" si="10"/>
         <v>Correct</v>
       </c>
       <c r="U7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="V7" s="36">
+      <c r="V7" s="11">
         <f>COUNTIF(R$4:R$14, "Correct") / COUNTA(R$4:R$14)</f>
         <v>0.81818181818181823</v>
       </c>
@@ -4132,7 +4123,7 @@
         <v>0.18181818181818182</v>
       </c>
       <c r="X7" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -4158,50 +4149,50 @@
       <c r="G8" s="11">
         <v>-0.54647684275259234</v>
       </c>
-      <c r="I8" s="29" t="str">
-        <f>IF(AND($B8&gt;0, C8&gt;0), "Q1", IF(AND($B8&lt;0, C8&gt;0), "Q2", IF(AND($B8&lt;0, C8&lt;0), "Q3", "Q4")))</f>
+      <c r="I8" s="28" t="str">
+        <f t="shared" si="0"/>
         <v>Q4</v>
       </c>
-      <c r="J8" s="29" t="str">
-        <f>IF(AND($B8&gt;0, D8&gt;0), "Q1", IF(AND($B8&lt;0, D8&gt;0), "Q2", IF(AND($B8&lt;0, D8&lt;0), "Q3", "Q4")))</f>
+      <c r="J8" s="28" t="str">
+        <f t="shared" si="1"/>
         <v>Q4</v>
       </c>
-      <c r="K8" s="29" t="str">
-        <f>IF(AND($B8&gt;0, E8&gt;0), "Q1", IF(AND($B8&lt;0, E8&gt;0), "Q2", IF(AND($B8&lt;0, E8&lt;0), "Q3", "Q4")))</f>
+      <c r="K8" s="28" t="str">
+        <f t="shared" si="2"/>
         <v>Q4</v>
       </c>
-      <c r="L8" s="29" t="str">
-        <f>IF(AND($B8&gt;0, F8&gt;0), "Q1", IF(AND($B8&lt;0, F8&gt;0), "Q2", IF(AND($B8&lt;0, F8&lt;0), "Q3", "Q4")))</f>
+      <c r="L8" s="28" t="str">
+        <f t="shared" si="3"/>
         <v>Q4</v>
       </c>
-      <c r="M8" s="29" t="str">
-        <f>IF(AND($B8&gt;0, G8&gt;0), "Q1", IF(AND($B8&lt;0, G8&gt;0), "Q2", IF(AND($B8&lt;0, G8&lt;0), "Q3", "Q4")))</f>
+      <c r="M8" s="28" t="str">
+        <f t="shared" si="4"/>
         <v>Q4</v>
       </c>
-      <c r="O8" s="29" t="str">
-        <f t="shared" si="1"/>
-        <v>Correct</v>
-      </c>
-      <c r="P8" s="29" t="str">
-        <f t="shared" si="2"/>
-        <v>Correct</v>
-      </c>
-      <c r="Q8" s="29" t="str">
-        <f t="shared" si="3"/>
-        <v>Correct</v>
-      </c>
-      <c r="R8" s="29" t="str">
-        <f t="shared" si="4"/>
-        <v>Correct</v>
-      </c>
-      <c r="S8" s="29" t="str">
-        <f t="shared" si="5"/>
+      <c r="O8" s="28" t="str">
+        <f t="shared" si="6"/>
+        <v>Correct</v>
+      </c>
+      <c r="P8" s="28" t="str">
+        <f t="shared" si="7"/>
+        <v>Correct</v>
+      </c>
+      <c r="Q8" s="28" t="str">
+        <f t="shared" si="8"/>
+        <v>Correct</v>
+      </c>
+      <c r="R8" s="28" t="str">
+        <f t="shared" si="9"/>
+        <v>Correct</v>
+      </c>
+      <c r="S8" s="28" t="str">
+        <f t="shared" si="10"/>
         <v>Correct</v>
       </c>
       <c r="U8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="V8" s="36">
+      <c r="V8" s="11">
         <f>COUNTIF(S$4:S$14, "Correct") / COUNTA(S$4:S$14)</f>
         <v>0.81818181818181823</v>
       </c>
@@ -4210,7 +4201,7 @@
         <v>0.18181818181818182</v>
       </c>
       <c r="X8" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -4236,44 +4227,44 @@
       <c r="G9" s="11">
         <v>-0.50628641399623708</v>
       </c>
-      <c r="I9" s="29" t="str">
-        <f>IF(AND($B9&gt;0, C9&gt;0), "Q1", IF(AND($B9&lt;0, C9&gt;0), "Q2", IF(AND($B9&lt;0, C9&lt;0), "Q3", "Q4")))</f>
+      <c r="I9" s="28" t="str">
+        <f t="shared" si="0"/>
         <v>Q4</v>
       </c>
-      <c r="J9" s="29" t="str">
-        <f>IF(AND($B9&gt;0, D9&gt;0), "Q1", IF(AND($B9&lt;0, D9&gt;0), "Q2", IF(AND($B9&lt;0, D9&lt;0), "Q3", "Q4")))</f>
+      <c r="J9" s="28" t="str">
+        <f t="shared" si="1"/>
         <v>Q4</v>
       </c>
-      <c r="K9" s="29" t="str">
-        <f>IF(AND($B9&gt;0, E9&gt;0), "Q1", IF(AND($B9&lt;0, E9&gt;0), "Q2", IF(AND($B9&lt;0, E9&lt;0), "Q3", "Q4")))</f>
+      <c r="K9" s="28" t="str">
+        <f t="shared" si="2"/>
         <v>Q4</v>
       </c>
-      <c r="L9" s="29" t="str">
-        <f>IF(AND($B9&gt;0, F9&gt;0), "Q1", IF(AND($B9&lt;0, F9&gt;0), "Q2", IF(AND($B9&lt;0, F9&lt;0), "Q3", "Q4")))</f>
+      <c r="L9" s="28" t="str">
+        <f t="shared" si="3"/>
         <v>Q4</v>
       </c>
-      <c r="M9" s="29" t="str">
-        <f>IF(AND($B9&gt;0, G9&gt;0), "Q1", IF(AND($B9&lt;0, G9&gt;0), "Q2", IF(AND($B9&lt;0, G9&lt;0), "Q3", "Q4")))</f>
+      <c r="M9" s="28" t="str">
+        <f t="shared" si="4"/>
         <v>Q4</v>
       </c>
-      <c r="O9" s="29" t="str">
-        <f t="shared" si="1"/>
-        <v>Correct</v>
-      </c>
-      <c r="P9" s="29" t="str">
-        <f t="shared" si="2"/>
-        <v>Correct</v>
-      </c>
-      <c r="Q9" s="29" t="str">
-        <f t="shared" si="3"/>
-        <v>Correct</v>
-      </c>
-      <c r="R9" s="29" t="str">
-        <f t="shared" si="4"/>
-        <v>Correct</v>
-      </c>
-      <c r="S9" s="29" t="str">
-        <f t="shared" si="5"/>
+      <c r="O9" s="28" t="str">
+        <f t="shared" si="6"/>
+        <v>Correct</v>
+      </c>
+      <c r="P9" s="28" t="str">
+        <f t="shared" si="7"/>
+        <v>Correct</v>
+      </c>
+      <c r="Q9" s="28" t="str">
+        <f t="shared" si="8"/>
+        <v>Correct</v>
+      </c>
+      <c r="R9" s="28" t="str">
+        <f t="shared" si="9"/>
+        <v>Correct</v>
+      </c>
+      <c r="S9" s="28" t="str">
+        <f t="shared" si="10"/>
         <v>Correct</v>
       </c>
     </row>
@@ -4299,44 +4290,44 @@
       <c r="G10" s="11">
         <v>-0.21932285347228794</v>
       </c>
-      <c r="I10" s="33" t="str">
-        <f>IF(AND($B10&gt;0, C10&gt;0), "Q1", IF(AND($B10&lt;0, C10&gt;0), "Q2", IF(AND($B10&lt;0, C10&lt;0), "Q3", "Q4")))</f>
+      <c r="I10" s="30" t="str">
+        <f t="shared" si="0"/>
         <v>Q3</v>
       </c>
-      <c r="J10" s="30" t="str">
-        <f>IF(AND($B10&gt;0, D10&gt;0), "Q1", IF(AND($B10&lt;0, D10&gt;0), "Q2", IF(AND($B10&lt;0, D10&lt;0), "Q3", "Q4")))</f>
+      <c r="J10" s="29" t="str">
+        <f t="shared" si="1"/>
         <v>Q2</v>
       </c>
-      <c r="K10" s="33" t="str">
-        <f>IF(AND($B10&gt;0, E10&gt;0), "Q1", IF(AND($B10&lt;0, E10&gt;0), "Q2", IF(AND($B10&lt;0, E10&lt;0), "Q3", "Q4")))</f>
+      <c r="K10" s="30" t="str">
+        <f t="shared" si="2"/>
         <v>Q3</v>
       </c>
-      <c r="L10" s="33" t="str">
-        <f>IF(AND($B10&gt;0, F10&gt;0), "Q1", IF(AND($B10&lt;0, F10&gt;0), "Q2", IF(AND($B10&lt;0, F10&lt;0), "Q3", "Q4")))</f>
+      <c r="L10" s="30" t="str">
+        <f t="shared" si="3"/>
         <v>Q3</v>
       </c>
-      <c r="M10" s="33" t="str">
-        <f>IF(AND($B10&gt;0, G10&gt;0), "Q1", IF(AND($B10&lt;0, G10&gt;0), "Q2", IF(AND($B10&lt;0, G10&lt;0), "Q3", "Q4")))</f>
+      <c r="M10" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>Q3</v>
       </c>
-      <c r="O10" s="34" t="str">
-        <f t="shared" si="1"/>
+      <c r="O10" s="31" t="str">
+        <f t="shared" si="6"/>
         <v>Incorrect</v>
       </c>
-      <c r="P10" s="29" t="str">
-        <f t="shared" si="2"/>
-        <v>Correct</v>
-      </c>
-      <c r="Q10" s="34" t="str">
-        <f t="shared" si="3"/>
+      <c r="P10" s="28" t="str">
+        <f t="shared" si="7"/>
+        <v>Correct</v>
+      </c>
+      <c r="Q10" s="31" t="str">
+        <f t="shared" si="8"/>
         <v>Incorrect</v>
       </c>
-      <c r="R10" s="34" t="str">
-        <f t="shared" si="4"/>
+      <c r="R10" s="31" t="str">
+        <f t="shared" si="9"/>
         <v>Incorrect</v>
       </c>
-      <c r="S10" s="34" t="str">
-        <f t="shared" si="5"/>
+      <c r="S10" s="31" t="str">
+        <f t="shared" si="10"/>
         <v>Incorrect</v>
       </c>
       <c r="V10" s="32" t="s">
@@ -4367,53 +4358,53 @@
       <c r="G11" s="11">
         <v>0.38197141359573233</v>
       </c>
-      <c r="I11" s="33" t="str">
-        <f>IF(AND($B11&gt;0, C11&gt;0), "Q1", IF(AND($B11&lt;0, C11&gt;0), "Q2", IF(AND($B11&lt;0, C11&lt;0), "Q3", "Q4")))</f>
+      <c r="I11" s="30" t="str">
+        <f t="shared" si="0"/>
         <v>Q3</v>
       </c>
-      <c r="J11" s="33" t="str">
-        <f>IF(AND($B11&gt;0, D11&gt;0), "Q1", IF(AND($B11&lt;0, D11&gt;0), "Q2", IF(AND($B11&lt;0, D11&lt;0), "Q3", "Q4")))</f>
+      <c r="J11" s="30" t="str">
+        <f t="shared" si="1"/>
         <v>Q3</v>
       </c>
-      <c r="K11" s="30" t="str">
-        <f>IF(AND($B11&gt;0, E11&gt;0), "Q1", IF(AND($B11&lt;0, E11&gt;0), "Q2", IF(AND($B11&lt;0, E11&lt;0), "Q3", "Q4")))</f>
+      <c r="K11" s="29" t="str">
+        <f t="shared" si="2"/>
         <v>Q2</v>
       </c>
-      <c r="L11" s="30" t="str">
-        <f>IF(AND($B11&gt;0, F11&gt;0), "Q1", IF(AND($B11&lt;0, F11&gt;0), "Q2", IF(AND($B11&lt;0, F11&lt;0), "Q3", "Q4")))</f>
+      <c r="L11" s="29" t="str">
+        <f t="shared" si="3"/>
         <v>Q2</v>
       </c>
-      <c r="M11" s="30" t="str">
-        <f>IF(AND($B11&gt;0, G11&gt;0), "Q1", IF(AND($B11&lt;0, G11&gt;0), "Q2", IF(AND($B11&lt;0, G11&lt;0), "Q3", "Q4")))</f>
+      <c r="M11" s="29" t="str">
+        <f t="shared" si="4"/>
         <v>Q2</v>
       </c>
-      <c r="O11" s="34" t="str">
-        <f t="shared" si="1"/>
+      <c r="O11" s="31" t="str">
+        <f t="shared" si="6"/>
         <v>Incorrect</v>
       </c>
-      <c r="P11" s="34" t="str">
-        <f t="shared" si="2"/>
+      <c r="P11" s="31" t="str">
+        <f t="shared" si="7"/>
         <v>Incorrect</v>
       </c>
-      <c r="Q11" s="29" t="str">
-        <f t="shared" si="3"/>
-        <v>Correct</v>
-      </c>
-      <c r="R11" s="29" t="str">
-        <f t="shared" si="4"/>
-        <v>Correct</v>
-      </c>
-      <c r="S11" s="29" t="str">
-        <f t="shared" si="5"/>
-        <v>Correct</v>
-      </c>
-      <c r="V11" s="35" t="s">
+      <c r="Q11" s="28" t="str">
+        <f t="shared" si="8"/>
+        <v>Correct</v>
+      </c>
+      <c r="R11" s="28" t="str">
+        <f t="shared" si="9"/>
+        <v>Correct</v>
+      </c>
+      <c r="S11" s="28" t="str">
+        <f t="shared" si="10"/>
+        <v>Correct</v>
+      </c>
+      <c r="V11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="W11" s="35" t="s">
+      <c r="W11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="X11" s="35" t="s">
+      <c r="X11" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -4439,54 +4430,54 @@
       <c r="G12" s="11">
         <v>1.0775013302402989</v>
       </c>
-      <c r="I12" s="30" t="str">
-        <f>IF(AND($B12&gt;0, C12&gt;0), "Q1", IF(AND($B12&lt;0, C12&gt;0), "Q2", IF(AND($B12&lt;0, C12&lt;0), "Q3", "Q4")))</f>
+      <c r="I12" s="29" t="str">
+        <f t="shared" si="0"/>
         <v>Q2</v>
       </c>
-      <c r="J12" s="30" t="str">
-        <f>IF(AND($B12&gt;0, D12&gt;0), "Q1", IF(AND($B12&lt;0, D12&gt;0), "Q2", IF(AND($B12&lt;0, D12&lt;0), "Q3", "Q4")))</f>
+      <c r="J12" s="29" t="str">
+        <f t="shared" si="1"/>
         <v>Q2</v>
       </c>
-      <c r="K12" s="30" t="str">
-        <f>IF(AND($B12&gt;0, E12&gt;0), "Q1", IF(AND($B12&lt;0, E12&gt;0), "Q2", IF(AND($B12&lt;0, E12&lt;0), "Q3", "Q4")))</f>
+      <c r="K12" s="29" t="str">
+        <f t="shared" si="2"/>
         <v>Q2</v>
       </c>
-      <c r="L12" s="30" t="str">
-        <f>IF(AND($B12&gt;0, F12&gt;0), "Q1", IF(AND($B12&lt;0, F12&gt;0), "Q2", IF(AND($B12&lt;0, F12&lt;0), "Q3", "Q4")))</f>
+      <c r="L12" s="29" t="str">
+        <f t="shared" si="3"/>
         <v>Q2</v>
       </c>
-      <c r="M12" s="30" t="str">
-        <f>IF(AND($B12&gt;0, G12&gt;0), "Q1", IF(AND($B12&lt;0, G12&gt;0), "Q2", IF(AND($B12&lt;0, G12&lt;0), "Q3", "Q4")))</f>
+      <c r="M12" s="29" t="str">
+        <f t="shared" si="4"/>
         <v>Q2</v>
       </c>
-      <c r="O12" s="29" t="str">
-        <f t="shared" si="1"/>
-        <v>Correct</v>
-      </c>
-      <c r="P12" s="29" t="str">
-        <f t="shared" si="2"/>
-        <v>Correct</v>
-      </c>
-      <c r="Q12" s="29" t="str">
-        <f t="shared" si="3"/>
-        <v>Correct</v>
-      </c>
-      <c r="R12" s="29" t="str">
-        <f t="shared" si="4"/>
-        <v>Correct</v>
-      </c>
-      <c r="S12" s="29" t="str">
-        <f t="shared" si="5"/>
+      <c r="O12" s="28" t="str">
+        <f t="shared" si="6"/>
+        <v>Correct</v>
+      </c>
+      <c r="P12" s="28" t="str">
+        <f t="shared" si="7"/>
+        <v>Correct</v>
+      </c>
+      <c r="Q12" s="28" t="str">
+        <f t="shared" si="8"/>
+        <v>Correct</v>
+      </c>
+      <c r="R12" s="28" t="str">
+        <f t="shared" si="9"/>
+        <v>Correct</v>
+      </c>
+      <c r="S12" s="28" t="str">
+        <f t="shared" si="10"/>
         <v>Correct</v>
       </c>
       <c r="U12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="V12" s="36">
+      <c r="V12" s="11">
         <f>COUNTIF(O$18:O$25, "Correct") / COUNTA(O$18:O$25)</f>
         <v>0.75</v>
       </c>
-      <c r="W12" s="36">
+      <c r="W12" s="11">
         <f>COUNTIF(O$18:O$25, "Incorrect") / COUNTA(O$18:O$25)</f>
         <v>0.25</v>
       </c>
@@ -4517,59 +4508,59 @@
       <c r="G13" s="11">
         <v>0.16781718326223696</v>
       </c>
-      <c r="I13" s="33" t="str">
-        <f>IF(AND($B13&gt;0, C13&gt;0), "Q1", IF(AND($B13&lt;0, C13&gt;0), "Q2", IF(AND($B13&lt;0, C13&lt;0), "Q3", "Q4")))</f>
+      <c r="I13" s="30" t="str">
+        <f t="shared" si="0"/>
         <v>Q3</v>
       </c>
-      <c r="J13" s="33" t="str">
-        <f>IF(AND($B13&gt;0, D13&gt;0), "Q1", IF(AND($B13&lt;0, D13&gt;0), "Q2", IF(AND($B13&lt;0, D13&lt;0), "Q3", "Q4")))</f>
+      <c r="J13" s="30" t="str">
+        <f t="shared" si="1"/>
         <v>Q3</v>
       </c>
-      <c r="K13" s="30" t="str">
-        <f>IF(AND($B13&gt;0, E13&gt;0), "Q1", IF(AND($B13&lt;0, E13&gt;0), "Q2", IF(AND($B13&lt;0, E13&lt;0), "Q3", "Q4")))</f>
+      <c r="K13" s="29" t="str">
+        <f t="shared" si="2"/>
         <v>Q2</v>
       </c>
-      <c r="L13" s="30" t="str">
-        <f>IF(AND($B13&gt;0, F13&gt;0), "Q1", IF(AND($B13&lt;0, F13&gt;0), "Q2", IF(AND($B13&lt;0, F13&lt;0), "Q3", "Q4")))</f>
+      <c r="L13" s="29" t="str">
+        <f t="shared" si="3"/>
         <v>Q2</v>
       </c>
-      <c r="M13" s="30" t="str">
-        <f>IF(AND($B13&gt;0, G13&gt;0), "Q1", IF(AND($B13&lt;0, G13&gt;0), "Q2", IF(AND($B13&lt;0, G13&lt;0), "Q3", "Q4")))</f>
+      <c r="M13" s="29" t="str">
+        <f t="shared" si="4"/>
         <v>Q2</v>
       </c>
-      <c r="O13" s="34" t="str">
-        <f t="shared" si="1"/>
+      <c r="O13" s="31" t="str">
+        <f t="shared" si="6"/>
         <v>Incorrect</v>
       </c>
-      <c r="P13" s="34" t="str">
-        <f t="shared" si="2"/>
+      <c r="P13" s="31" t="str">
+        <f t="shared" si="7"/>
         <v>Incorrect</v>
       </c>
-      <c r="Q13" s="29" t="str">
-        <f t="shared" si="3"/>
-        <v>Correct</v>
-      </c>
-      <c r="R13" s="29" t="str">
-        <f t="shared" si="4"/>
-        <v>Correct</v>
-      </c>
-      <c r="S13" s="29" t="str">
-        <f t="shared" si="5"/>
+      <c r="Q13" s="28" t="str">
+        <f t="shared" si="8"/>
+        <v>Correct</v>
+      </c>
+      <c r="R13" s="28" t="str">
+        <f t="shared" si="9"/>
+        <v>Correct</v>
+      </c>
+      <c r="S13" s="28" t="str">
+        <f t="shared" si="10"/>
         <v>Correct</v>
       </c>
       <c r="U13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="V13" s="36">
+      <c r="V13" s="11">
         <f>COUNTIF(P$18:P$25, "Correct") / COUNTA(P$18:P$25)</f>
         <v>0.5</v>
       </c>
-      <c r="W13" s="36">
+      <c r="W13" s="11">
         <f>COUNTIF(P$18:P$25, "Incorrect") / COUNTA(P$18:P$25)</f>
         <v>0.5</v>
       </c>
       <c r="X13" s="10">
-        <f t="shared" ref="X13:X16" si="7">SUM(V13:W13)</f>
+        <f t="shared" ref="X13:X16" si="12">SUM(V13:W13)</f>
         <v>1</v>
       </c>
     </row>
@@ -4595,59 +4586,59 @@
       <c r="G14" s="11">
         <v>-0.21328231594690392</v>
       </c>
-      <c r="I14" s="33" t="str">
-        <f>IF(AND($B14&gt;0, C14&gt;0), "Q1", IF(AND($B14&lt;0, C14&gt;0), "Q2", IF(AND($B14&lt;0, C14&lt;0), "Q3", "Q4")))</f>
+      <c r="I14" s="30" t="str">
+        <f t="shared" si="0"/>
         <v>Q3</v>
       </c>
-      <c r="J14" s="33" t="str">
-        <f>IF(AND($B14&gt;0, D14&gt;0), "Q1", IF(AND($B14&lt;0, D14&gt;0), "Q2", IF(AND($B14&lt;0, D14&lt;0), "Q3", "Q4")))</f>
+      <c r="J14" s="30" t="str">
+        <f t="shared" si="1"/>
         <v>Q3</v>
       </c>
-      <c r="K14" s="33" t="str">
-        <f>IF(AND($B14&gt;0, E14&gt;0), "Q1", IF(AND($B14&lt;0, E14&gt;0), "Q2", IF(AND($B14&lt;0, E14&lt;0), "Q3", "Q4")))</f>
+      <c r="K14" s="30" t="str">
+        <f t="shared" si="2"/>
         <v>Q3</v>
       </c>
-      <c r="L14" s="33" t="str">
-        <f>IF(AND($B14&gt;0, F14&gt;0), "Q1", IF(AND($B14&lt;0, F14&gt;0), "Q2", IF(AND($B14&lt;0, F14&lt;0), "Q3", "Q4")))</f>
+      <c r="L14" s="30" t="str">
+        <f t="shared" si="3"/>
         <v>Q3</v>
       </c>
-      <c r="M14" s="33" t="str">
-        <f>IF(AND($B14&gt;0, G14&gt;0), "Q1", IF(AND($B14&lt;0, G14&gt;0), "Q2", IF(AND($B14&lt;0, G14&lt;0), "Q3", "Q4")))</f>
+      <c r="M14" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>Q3</v>
       </c>
-      <c r="O14" s="34" t="str">
-        <f t="shared" si="1"/>
+      <c r="O14" s="31" t="str">
+        <f t="shared" si="6"/>
         <v>Incorrect</v>
       </c>
-      <c r="P14" s="34" t="str">
-        <f t="shared" si="2"/>
+      <c r="P14" s="31" t="str">
+        <f t="shared" si="7"/>
         <v>Incorrect</v>
       </c>
-      <c r="Q14" s="34" t="str">
-        <f t="shared" si="3"/>
+      <c r="Q14" s="31" t="str">
+        <f t="shared" si="8"/>
         <v>Incorrect</v>
       </c>
-      <c r="R14" s="34" t="str">
-        <f t="shared" si="4"/>
+      <c r="R14" s="31" t="str">
+        <f t="shared" si="9"/>
         <v>Incorrect</v>
       </c>
-      <c r="S14" s="34" t="str">
-        <f t="shared" si="5"/>
+      <c r="S14" s="31" t="str">
+        <f t="shared" si="10"/>
         <v>Incorrect</v>
       </c>
       <c r="U14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="V14" s="36">
+      <c r="V14" s="11">
         <f>COUNTIF(Q$18:Q$25, "Correct") / COUNTA(Q$18:Q$25)</f>
         <v>0.75</v>
       </c>
-      <c r="W14" s="36">
+      <c r="W14" s="11">
         <f>COUNTIF(Q$18:Q$25, "Incorrect") / COUNTA(Q$18:Q$25)</f>
         <v>0.25</v>
       </c>
       <c r="X14" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -4655,54 +4646,54 @@
       <c r="U15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="V15" s="36">
+      <c r="V15" s="11">
         <f>COUNTIF(R$18:R$25, "Correct") / COUNTA(R$18:R$25)</f>
         <v>0.625</v>
       </c>
-      <c r="W15" s="36">
+      <c r="W15" s="11">
         <f>COUNTIF(R$18:R$25, "Incorrect") / COUNTA(R$18:R$25)</f>
         <v>0.375</v>
       </c>
       <c r="X15" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="I16" s="31" t="s">
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="I16" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="J16" s="31"/>
-      <c r="K16" s="31"/>
-      <c r="L16" s="31"/>
-      <c r="M16" s="31"/>
-      <c r="O16" s="23" t="s">
+      <c r="J16" s="33"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="33"/>
+      <c r="M16" s="33"/>
+      <c r="O16" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="23"/>
-      <c r="S16" s="23"/>
+      <c r="P16" s="33"/>
+      <c r="Q16" s="33"/>
+      <c r="R16" s="33"/>
+      <c r="S16" s="33"/>
       <c r="U16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="V16" s="36">
+      <c r="V16" s="11">
         <f>COUNTIF(S$18:S$25, "Correct") / COUNTA(S$18:S$25)</f>
         <v>1</v>
       </c>
-      <c r="W16" s="36">
+      <c r="W16" s="11">
         <f>COUNTIF(S$18:S$25, "Incorrect") / COUNTA(S$18:S$25)</f>
         <v>0</v>
       </c>
       <c r="X16" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -4766,7 +4757,7 @@
       <c r="B18" s="19">
         <v>-0.10058679002726996</v>
       </c>
-      <c r="C18" s="25">
+      <c r="C18" s="24">
         <v>0.10636991288633117</v>
       </c>
       <c r="D18" s="11">
@@ -4781,44 +4772,44 @@
       <c r="G18" s="11">
         <v>0.18061966240201743</v>
       </c>
-      <c r="I18" s="29" t="str">
-        <f>IF(AND($B18&gt;0, C18&gt;0), "Q1", IF(AND($B18&lt;0, C18&gt;0), "Q2", IF(AND($B18&lt;0, C18&lt;0), "Q3", "Q4")))</f>
+      <c r="I18" s="28" t="str">
+        <f t="shared" ref="I18:M25" si="13">IF(AND($B18&gt;0, C18&gt;0), "Q1", IF(AND($B18&lt;0, C18&gt;0), "Q2", IF(AND($B18&lt;0, C18&lt;0), "Q3", "Q4")))</f>
         <v>Q2</v>
       </c>
-      <c r="J18" s="29" t="str">
-        <f>IF(AND($B18&gt;0, D18&gt;0), "Q1", IF(AND($B18&lt;0, D18&gt;0), "Q2", IF(AND($B18&lt;0, D18&lt;0), "Q3", "Q4")))</f>
+      <c r="J18" s="28" t="str">
+        <f t="shared" si="13"/>
         <v>Q2</v>
       </c>
-      <c r="K18" s="29" t="str">
-        <f>IF(AND($B18&gt;0, E18&gt;0), "Q1", IF(AND($B18&lt;0, E18&gt;0), "Q2", IF(AND($B18&lt;0, E18&lt;0), "Q3", "Q4")))</f>
+      <c r="K18" s="28" t="str">
+        <f t="shared" si="13"/>
         <v>Q2</v>
       </c>
-      <c r="L18" s="29" t="str">
-        <f>IF(AND($B18&gt;0, F18&gt;0), "Q1", IF(AND($B18&lt;0, F18&gt;0), "Q2", IF(AND($B18&lt;0, F18&lt;0), "Q3", "Q4")))</f>
+      <c r="L18" s="28" t="str">
+        <f t="shared" si="13"/>
         <v>Q2</v>
       </c>
-      <c r="M18" s="29" t="str">
-        <f>IF(AND($B18&gt;0, G18&gt;0), "Q1", IF(AND($B18&lt;0, G18&gt;0), "Q2", IF(AND($B18&lt;0, G18&lt;0), "Q3", "Q4")))</f>
+      <c r="M18" s="28" t="str">
+        <f t="shared" si="13"/>
         <v>Q2</v>
       </c>
-      <c r="O18" s="29" t="str">
+      <c r="O18" s="28" t="str">
         <f>IF(OR(I18="Q2", I18="Q4"), "Correct", "Incorrect")</f>
         <v>Correct</v>
       </c>
-      <c r="P18" s="29" t="str">
-        <f t="shared" ref="P18:S18" si="8">IF(OR(J18="Q2", J18="Q4"), "Correct", "Incorrect")</f>
-        <v>Correct</v>
-      </c>
-      <c r="Q18" s="29" t="str">
-        <f t="shared" si="8"/>
-        <v>Correct</v>
-      </c>
-      <c r="R18" s="29" t="str">
-        <f t="shared" si="8"/>
-        <v>Correct</v>
-      </c>
-      <c r="S18" s="29" t="str">
-        <f t="shared" si="8"/>
+      <c r="P18" s="28" t="str">
+        <f t="shared" ref="P18:S18" si="14">IF(OR(J18="Q2", J18="Q4"), "Correct", "Incorrect")</f>
+        <v>Correct</v>
+      </c>
+      <c r="Q18" s="28" t="str">
+        <f t="shared" si="14"/>
+        <v>Correct</v>
+      </c>
+      <c r="R18" s="28" t="str">
+        <f t="shared" si="14"/>
+        <v>Correct</v>
+      </c>
+      <c r="S18" s="28" t="str">
+        <f t="shared" si="14"/>
         <v>Correct</v>
       </c>
     </row>
@@ -4829,7 +4820,7 @@
       <c r="B19" s="20">
         <v>-0.32001589401318453</v>
       </c>
-      <c r="C19" s="26">
+      <c r="C19" s="25">
         <v>0.46884704968944091</v>
       </c>
       <c r="D19" s="11">
@@ -4844,44 +4835,44 @@
       <c r="G19" s="11">
         <v>0.25528328492852753</v>
       </c>
-      <c r="I19" s="29" t="str">
-        <f>IF(AND($B19&gt;0, C19&gt;0), "Q1", IF(AND($B19&lt;0, C19&gt;0), "Q2", IF(AND($B19&lt;0, C19&lt;0), "Q3", "Q4")))</f>
+      <c r="I19" s="28" t="str">
+        <f t="shared" si="13"/>
         <v>Q2</v>
       </c>
-      <c r="J19" s="29" t="str">
-        <f>IF(AND($B19&gt;0, D19&gt;0), "Q1", IF(AND($B19&lt;0, D19&gt;0), "Q2", IF(AND($B19&lt;0, D19&lt;0), "Q3", "Q4")))</f>
+      <c r="J19" s="28" t="str">
+        <f t="shared" si="13"/>
         <v>Q2</v>
       </c>
-      <c r="K19" s="29" t="str">
-        <f>IF(AND($B19&gt;0, E19&gt;0), "Q1", IF(AND($B19&lt;0, E19&gt;0), "Q2", IF(AND($B19&lt;0, E19&lt;0), "Q3", "Q4")))</f>
+      <c r="K19" s="28" t="str">
+        <f t="shared" si="13"/>
         <v>Q2</v>
       </c>
-      <c r="L19" s="29" t="str">
-        <f>IF(AND($B19&gt;0, F19&gt;0), "Q1", IF(AND($B19&lt;0, F19&gt;0), "Q2", IF(AND($B19&lt;0, F19&lt;0), "Q3", "Q4")))</f>
+      <c r="L19" s="28" t="str">
+        <f t="shared" si="13"/>
         <v>Q2</v>
       </c>
-      <c r="M19" s="29" t="str">
-        <f>IF(AND($B19&gt;0, G19&gt;0), "Q1", IF(AND($B19&lt;0, G19&gt;0), "Q2", IF(AND($B19&lt;0, G19&lt;0), "Q3", "Q4")))</f>
+      <c r="M19" s="28" t="str">
+        <f t="shared" si="13"/>
         <v>Q2</v>
       </c>
-      <c r="O19" s="29" t="str">
-        <f t="shared" ref="O19:O25" si="9">IF(OR(I19="Q2", I19="Q4"), "Correct", "Incorrect")</f>
-        <v>Correct</v>
-      </c>
-      <c r="P19" s="29" t="str">
-        <f t="shared" ref="P19:P25" si="10">IF(OR(J19="Q2", J19="Q4"), "Correct", "Incorrect")</f>
-        <v>Correct</v>
-      </c>
-      <c r="Q19" s="29" t="str">
-        <f t="shared" ref="Q19:Q25" si="11">IF(OR(K19="Q2", K19="Q4"), "Correct", "Incorrect")</f>
-        <v>Correct</v>
-      </c>
-      <c r="R19" s="29" t="str">
-        <f t="shared" ref="R19:R25" si="12">IF(OR(L19="Q2", L19="Q4"), "Correct", "Incorrect")</f>
-        <v>Correct</v>
-      </c>
-      <c r="S19" s="29" t="str">
-        <f t="shared" ref="S19:S25" si="13">IF(OR(M19="Q2", M19="Q4"), "Correct", "Incorrect")</f>
+      <c r="O19" s="28" t="str">
+        <f t="shared" ref="O19:O25" si="15">IF(OR(I19="Q2", I19="Q4"), "Correct", "Incorrect")</f>
+        <v>Correct</v>
+      </c>
+      <c r="P19" s="28" t="str">
+        <f t="shared" ref="P19:P25" si="16">IF(OR(J19="Q2", J19="Q4"), "Correct", "Incorrect")</f>
+        <v>Correct</v>
+      </c>
+      <c r="Q19" s="28" t="str">
+        <f t="shared" ref="Q19:Q25" si="17">IF(OR(K19="Q2", K19="Q4"), "Correct", "Incorrect")</f>
+        <v>Correct</v>
+      </c>
+      <c r="R19" s="28" t="str">
+        <f t="shared" ref="R19:R25" si="18">IF(OR(L19="Q2", L19="Q4"), "Correct", "Incorrect")</f>
+        <v>Correct</v>
+      </c>
+      <c r="S19" s="28" t="str">
+        <f t="shared" ref="S19:S24" si="19">IF(OR(M19="Q2", M19="Q4"), "Correct", "Incorrect")</f>
         <v>Correct</v>
       </c>
     </row>
@@ -4892,7 +4883,7 @@
       <c r="B20" s="21">
         <v>0.11743877238132332</v>
       </c>
-      <c r="C20" s="27">
+      <c r="C20" s="26">
         <v>-0.25624269896262869</v>
       </c>
       <c r="D20" s="11">
@@ -4907,44 +4898,44 @@
       <c r="G20" s="11">
         <v>-0.2142122573951242</v>
       </c>
-      <c r="I20" s="30" t="str">
-        <f>IF(AND($B20&gt;0, C20&gt;0), "Q1", IF(AND($B20&lt;0, C20&gt;0), "Q2", IF(AND($B20&lt;0, C20&lt;0), "Q3", "Q4")))</f>
+      <c r="I20" s="29" t="str">
+        <f t="shared" si="13"/>
         <v>Q4</v>
       </c>
-      <c r="J20" s="30" t="str">
-        <f>IF(AND($B20&gt;0, D20&gt;0), "Q1", IF(AND($B20&lt;0, D20&gt;0), "Q2", IF(AND($B20&lt;0, D20&lt;0), "Q3", "Q4")))</f>
+      <c r="J20" s="29" t="str">
+        <f t="shared" si="13"/>
         <v>Q4</v>
       </c>
-      <c r="K20" s="30" t="str">
-        <f>IF(AND($B20&gt;0, E20&gt;0), "Q1", IF(AND($B20&lt;0, E20&gt;0), "Q2", IF(AND($B20&lt;0, E20&lt;0), "Q3", "Q4")))</f>
+      <c r="K20" s="29" t="str">
+        <f t="shared" si="13"/>
         <v>Q4</v>
       </c>
-      <c r="L20" s="30" t="str">
-        <f>IF(AND($B20&gt;0, F20&gt;0), "Q1", IF(AND($B20&lt;0, F20&gt;0), "Q2", IF(AND($B20&lt;0, F20&lt;0), "Q3", "Q4")))</f>
+      <c r="L20" s="29" t="str">
+        <f t="shared" si="13"/>
         <v>Q4</v>
       </c>
-      <c r="M20" s="30" t="str">
-        <f>IF(AND($B20&gt;0, G20&gt;0), "Q1", IF(AND($B20&lt;0, G20&gt;0), "Q2", IF(AND($B20&lt;0, G20&lt;0), "Q3", "Q4")))</f>
+      <c r="M20" s="29" t="str">
+        <f t="shared" si="13"/>
         <v>Q4</v>
       </c>
-      <c r="O20" s="29" t="str">
-        <f t="shared" si="9"/>
-        <v>Correct</v>
-      </c>
-      <c r="P20" s="29" t="str">
-        <f t="shared" si="10"/>
-        <v>Correct</v>
-      </c>
-      <c r="Q20" s="29" t="str">
-        <f t="shared" si="11"/>
-        <v>Correct</v>
-      </c>
-      <c r="R20" s="29" t="str">
-        <f t="shared" si="12"/>
-        <v>Correct</v>
-      </c>
-      <c r="S20" s="29" t="str">
-        <f t="shared" si="13"/>
+      <c r="O20" s="28" t="str">
+        <f t="shared" si="15"/>
+        <v>Correct</v>
+      </c>
+      <c r="P20" s="28" t="str">
+        <f t="shared" si="16"/>
+        <v>Correct</v>
+      </c>
+      <c r="Q20" s="28" t="str">
+        <f t="shared" si="17"/>
+        <v>Correct</v>
+      </c>
+      <c r="R20" s="28" t="str">
+        <f t="shared" si="18"/>
+        <v>Correct</v>
+      </c>
+      <c r="S20" s="28" t="str">
+        <f t="shared" si="19"/>
         <v>Correct</v>
       </c>
     </row>
@@ -4955,7 +4946,7 @@
       <c r="B21" s="21">
         <v>0.11743877238132332</v>
       </c>
-      <c r="C21" s="27">
+      <c r="C21" s="26">
         <v>-0.3234573572194151</v>
       </c>
       <c r="D21" s="11">
@@ -4970,44 +4961,44 @@
       <c r="G21" s="11">
         <v>-0.12091619396052281</v>
       </c>
-      <c r="I21" s="30" t="str">
-        <f>IF(AND($B21&gt;0, C21&gt;0), "Q1", IF(AND($B21&lt;0, C21&gt;0), "Q2", IF(AND($B21&lt;0, C21&lt;0), "Q3", "Q4")))</f>
+      <c r="I21" s="29" t="str">
+        <f t="shared" si="13"/>
         <v>Q4</v>
       </c>
-      <c r="J21" s="30" t="str">
-        <f>IF(AND($B21&gt;0, D21&gt;0), "Q1", IF(AND($B21&lt;0, D21&gt;0), "Q2", IF(AND($B21&lt;0, D21&lt;0), "Q3", "Q4")))</f>
+      <c r="J21" s="29" t="str">
+        <f t="shared" si="13"/>
         <v>Q4</v>
       </c>
-      <c r="K21" s="30" t="str">
-        <f>IF(AND($B21&gt;0, E21&gt;0), "Q1", IF(AND($B21&lt;0, E21&gt;0), "Q2", IF(AND($B21&lt;0, E21&lt;0), "Q3", "Q4")))</f>
+      <c r="K21" s="29" t="str">
+        <f t="shared" si="13"/>
         <v>Q1</v>
       </c>
-      <c r="L21" s="30" t="str">
-        <f>IF(AND($B21&gt;0, F21&gt;0), "Q1", IF(AND($B21&lt;0, F21&gt;0), "Q2", IF(AND($B21&lt;0, F21&lt;0), "Q3", "Q4")))</f>
+      <c r="L21" s="29" t="str">
+        <f t="shared" si="13"/>
         <v>Q1</v>
       </c>
-      <c r="M21" s="30" t="str">
-        <f>IF(AND($B21&gt;0, G21&gt;0), "Q1", IF(AND($B21&lt;0, G21&gt;0), "Q2", IF(AND($B21&lt;0, G21&lt;0), "Q3", "Q4")))</f>
+      <c r="M21" s="29" t="str">
+        <f t="shared" si="13"/>
         <v>Q4</v>
       </c>
-      <c r="O21" s="29" t="str">
-        <f t="shared" si="9"/>
-        <v>Correct</v>
-      </c>
-      <c r="P21" s="29" t="str">
-        <f t="shared" si="10"/>
-        <v>Correct</v>
-      </c>
-      <c r="Q21" s="29" t="str">
-        <f t="shared" si="11"/>
+      <c r="O21" s="28" t="str">
+        <f t="shared" si="15"/>
+        <v>Correct</v>
+      </c>
+      <c r="P21" s="28" t="str">
+        <f t="shared" si="16"/>
+        <v>Correct</v>
+      </c>
+      <c r="Q21" s="28" t="str">
+        <f t="shared" si="17"/>
         <v>Incorrect</v>
       </c>
-      <c r="R21" s="29" t="str">
-        <f t="shared" si="12"/>
+      <c r="R21" s="28" t="str">
+        <f t="shared" si="18"/>
         <v>Incorrect</v>
       </c>
-      <c r="S21" s="29" t="str">
-        <f t="shared" si="13"/>
+      <c r="S21" s="28" t="str">
+        <f t="shared" si="19"/>
         <v>Correct</v>
       </c>
     </row>
@@ -5018,7 +5009,7 @@
       <c r="B22" s="17">
         <v>-4.5718099286610456E-2</v>
       </c>
-      <c r="C22" s="28">
+      <c r="C22" s="27">
         <v>-0.41374386493899812</v>
       </c>
       <c r="D22" s="11">
@@ -5033,44 +5024,44 @@
       <c r="G22" s="11">
         <v>0.19235164956740658</v>
       </c>
-      <c r="I22" s="33" t="str">
-        <f>IF(AND($B22&gt;0, C22&gt;0), "Q1", IF(AND($B22&lt;0, C22&gt;0), "Q2", IF(AND($B22&lt;0, C22&lt;0), "Q3", "Q4")))</f>
+      <c r="I22" s="30" t="str">
+        <f t="shared" si="13"/>
         <v>Q3</v>
       </c>
-      <c r="J22" s="33" t="str">
-        <f>IF(AND($B22&gt;0, D22&gt;0), "Q1", IF(AND($B22&lt;0, D22&gt;0), "Q2", IF(AND($B22&lt;0, D22&lt;0), "Q3", "Q4")))</f>
+      <c r="J22" s="30" t="str">
+        <f t="shared" si="13"/>
         <v>Q3</v>
       </c>
-      <c r="K22" s="29" t="str">
-        <f>IF(AND($B22&gt;0, E22&gt;0), "Q1", IF(AND($B22&lt;0, E22&gt;0), "Q2", IF(AND($B22&lt;0, E22&lt;0), "Q3", "Q4")))</f>
+      <c r="K22" s="28" t="str">
+        <f t="shared" si="13"/>
         <v>Q2</v>
       </c>
-      <c r="L22" s="29" t="str">
-        <f>IF(AND($B22&gt;0, F22&gt;0), "Q1", IF(AND($B22&lt;0, F22&gt;0), "Q2", IF(AND($B22&lt;0, F22&lt;0), "Q3", "Q4")))</f>
+      <c r="L22" s="28" t="str">
+        <f t="shared" si="13"/>
         <v>Q2</v>
       </c>
-      <c r="M22" s="29" t="str">
-        <f>IF(AND($B22&gt;0, G22&gt;0), "Q1", IF(AND($B22&lt;0, G22&gt;0), "Q2", IF(AND($B22&lt;0, G22&lt;0), "Q3", "Q4")))</f>
+      <c r="M22" s="28" t="str">
+        <f t="shared" si="13"/>
         <v>Q2</v>
       </c>
-      <c r="O22" s="34" t="str">
-        <f t="shared" si="9"/>
+      <c r="O22" s="31" t="str">
+        <f t="shared" si="15"/>
         <v>Incorrect</v>
       </c>
-      <c r="P22" s="34" t="str">
-        <f t="shared" si="10"/>
+      <c r="P22" s="31" t="str">
+        <f t="shared" si="16"/>
         <v>Incorrect</v>
       </c>
-      <c r="Q22" s="29" t="str">
-        <f t="shared" si="11"/>
-        <v>Correct</v>
-      </c>
-      <c r="R22" s="29" t="str">
-        <f t="shared" si="12"/>
-        <v>Correct</v>
-      </c>
-      <c r="S22" s="29" t="str">
-        <f t="shared" si="13"/>
+      <c r="Q22" s="28" t="str">
+        <f t="shared" si="17"/>
+        <v>Correct</v>
+      </c>
+      <c r="R22" s="28" t="str">
+        <f t="shared" si="18"/>
+        <v>Correct</v>
+      </c>
+      <c r="S22" s="28" t="str">
+        <f t="shared" si="19"/>
         <v>Correct</v>
       </c>
     </row>
@@ -5081,7 +5072,7 @@
       <c r="B23" s="20">
         <v>-0.11251612892623995</v>
       </c>
-      <c r="C23" s="26">
+      <c r="C23" s="25">
         <v>2.567973467663719E-2</v>
       </c>
       <c r="D23" s="11">
@@ -5096,44 +5087,44 @@
       <c r="G23" s="11">
         <v>6.9338931211544927E-2</v>
       </c>
-      <c r="I23" s="29" t="str">
-        <f>IF(AND($B23&gt;0, C23&gt;0), "Q1", IF(AND($B23&lt;0, C23&gt;0), "Q2", IF(AND($B23&lt;0, C23&lt;0), "Q3", "Q4")))</f>
+      <c r="I23" s="28" t="str">
+        <f t="shared" si="13"/>
         <v>Q2</v>
       </c>
-      <c r="J23" s="33" t="str">
-        <f>IF(AND($B23&gt;0, D23&gt;0), "Q1", IF(AND($B23&lt;0, D23&gt;0), "Q2", IF(AND($B23&lt;0, D23&lt;0), "Q3", "Q4")))</f>
+      <c r="J23" s="30" t="str">
+        <f t="shared" si="13"/>
         <v>Q3</v>
       </c>
-      <c r="K23" s="29" t="str">
-        <f>IF(AND($B23&gt;0, E23&gt;0), "Q1", IF(AND($B23&lt;0, E23&gt;0), "Q2", IF(AND($B23&lt;0, E23&lt;0), "Q3", "Q4")))</f>
+      <c r="K23" s="28" t="str">
+        <f t="shared" si="13"/>
         <v>Q2</v>
       </c>
-      <c r="L23" s="29" t="str">
-        <f>IF(AND($B23&gt;0, F23&gt;0), "Q1", IF(AND($B23&lt;0, F23&gt;0), "Q2", IF(AND($B23&lt;0, F23&lt;0), "Q3", "Q4")))</f>
+      <c r="L23" s="28" t="str">
+        <f t="shared" si="13"/>
         <v>Q3</v>
       </c>
-      <c r="M23" s="29" t="str">
-        <f>IF(AND($B23&gt;0, G23&gt;0), "Q1", IF(AND($B23&lt;0, G23&gt;0), "Q2", IF(AND($B23&lt;0, G23&lt;0), "Q3", "Q4")))</f>
+      <c r="M23" s="28" t="str">
+        <f t="shared" si="13"/>
         <v>Q2</v>
       </c>
-      <c r="O23" s="29" t="str">
-        <f t="shared" si="9"/>
-        <v>Correct</v>
-      </c>
-      <c r="P23" s="34" t="str">
-        <f t="shared" si="10"/>
+      <c r="O23" s="28" t="str">
+        <f t="shared" si="15"/>
+        <v>Correct</v>
+      </c>
+      <c r="P23" s="31" t="str">
+        <f t="shared" si="16"/>
         <v>Incorrect</v>
       </c>
-      <c r="Q23" s="29" t="str">
-        <f t="shared" si="11"/>
-        <v>Correct</v>
-      </c>
-      <c r="R23" s="29" t="str">
-        <f t="shared" si="12"/>
+      <c r="Q23" s="28" t="str">
+        <f t="shared" si="17"/>
+        <v>Correct</v>
+      </c>
+      <c r="R23" s="28" t="str">
+        <f t="shared" si="18"/>
         <v>Incorrect</v>
       </c>
-      <c r="S23" s="29" t="str">
-        <f t="shared" si="13"/>
+      <c r="S23" s="28" t="str">
+        <f t="shared" si="19"/>
         <v>Correct</v>
       </c>
     </row>
@@ -5144,7 +5135,7 @@
       <c r="B24" s="20">
         <v>-0.11251612892623995</v>
       </c>
-      <c r="C24" s="26">
+      <c r="C24" s="25">
         <v>-0.22271423175524177</v>
       </c>
       <c r="D24" s="11">
@@ -5159,44 +5150,44 @@
       <c r="G24" s="11">
         <v>0.30506992688237528</v>
       </c>
-      <c r="I24" s="33" t="str">
-        <f>IF(AND($B24&gt;0, C24&gt;0), "Q1", IF(AND($B24&lt;0, C24&gt;0), "Q2", IF(AND($B24&lt;0, C24&lt;0), "Q3", "Q4")))</f>
+      <c r="I24" s="30" t="str">
+        <f t="shared" si="13"/>
         <v>Q3</v>
       </c>
-      <c r="J24" s="33" t="str">
-        <f>IF(AND($B24&gt;0, D24&gt;0), "Q1", IF(AND($B24&lt;0, D24&gt;0), "Q2", IF(AND($B24&lt;0, D24&lt;0), "Q3", "Q4")))</f>
+      <c r="J24" s="30" t="str">
+        <f t="shared" si="13"/>
         <v>Q3</v>
       </c>
-      <c r="K24" s="33" t="str">
-        <f>IF(AND($B24&gt;0, E24&gt;0), "Q1", IF(AND($B24&lt;0, E24&gt;0), "Q2", IF(AND($B24&lt;0, E24&lt;0), "Q3", "Q4")))</f>
+      <c r="K24" s="30" t="str">
+        <f t="shared" si="13"/>
         <v>Q3</v>
       </c>
-      <c r="L24" s="33" t="str">
-        <f>IF(AND($B24&gt;0, F24&gt;0), "Q1", IF(AND($B24&lt;0, F24&gt;0), "Q2", IF(AND($B24&lt;0, F24&lt;0), "Q3", "Q4")))</f>
+      <c r="L24" s="30" t="str">
+        <f t="shared" si="13"/>
         <v>Q3</v>
       </c>
-      <c r="M24" s="29" t="str">
-        <f>IF(AND($B24&gt;0, G24&gt;0), "Q1", IF(AND($B24&lt;0, G24&gt;0), "Q2", IF(AND($B24&lt;0, G24&lt;0), "Q3", "Q4")))</f>
+      <c r="M24" s="28" t="str">
+        <f t="shared" si="13"/>
         <v>Q2</v>
       </c>
-      <c r="O24" s="34" t="str">
-        <f t="shared" si="9"/>
+      <c r="O24" s="31" t="str">
+        <f t="shared" si="15"/>
         <v>Incorrect</v>
       </c>
-      <c r="P24" s="34" t="str">
-        <f t="shared" si="10"/>
+      <c r="P24" s="31" t="str">
+        <f t="shared" si="16"/>
         <v>Incorrect</v>
       </c>
-      <c r="Q24" s="34" t="str">
-        <f t="shared" si="11"/>
+      <c r="Q24" s="31" t="str">
+        <f t="shared" si="17"/>
         <v>Incorrect</v>
       </c>
-      <c r="R24" s="34" t="str">
-        <f t="shared" si="12"/>
+      <c r="R24" s="31" t="str">
+        <f t="shared" si="18"/>
         <v>Incorrect</v>
       </c>
-      <c r="S24" s="29" t="str">
-        <f t="shared" si="13"/>
+      <c r="S24" s="28" t="str">
+        <f t="shared" si="19"/>
         <v>Correct</v>
       </c>
     </row>
@@ -5207,7 +5198,7 @@
       <c r="B25" s="22">
         <v>-4.9570413884485784E-2</v>
       </c>
-      <c r="C25" s="25">
+      <c r="C25" s="24">
         <v>1.3785509799603692E-2</v>
       </c>
       <c r="D25" s="11">
@@ -5222,43 +5213,43 @@
       <c r="G25" s="11">
         <v>0.73881089123312471</v>
       </c>
-      <c r="I25" s="29" t="str">
-        <f>IF(AND($B25&gt;0, C25&gt;0), "Q1", IF(AND($B25&lt;0, C25&gt;0), "Q2", IF(AND($B25&lt;0, C25&lt;0), "Q3", "Q4")))</f>
+      <c r="I25" s="28" t="str">
+        <f t="shared" si="13"/>
         <v>Q2</v>
       </c>
-      <c r="J25" s="33" t="str">
-        <f>IF(AND($B25&gt;0, D25&gt;0), "Q1", IF(AND($B25&lt;0, D25&gt;0), "Q2", IF(AND($B25&lt;0, D25&lt;0), "Q3", "Q4")))</f>
+      <c r="J25" s="30" t="str">
+        <f t="shared" si="13"/>
         <v>Q3</v>
       </c>
-      <c r="K25" s="29" t="str">
-        <f>IF(AND($B25&gt;0, E25&gt;0), "Q1", IF(AND($B25&lt;0, E25&gt;0), "Q2", IF(AND($B25&lt;0, E25&lt;0), "Q3", "Q4")))</f>
+      <c r="K25" s="28" t="str">
+        <f t="shared" si="13"/>
         <v>Q2</v>
       </c>
-      <c r="L25" s="29" t="str">
-        <f>IF(AND($B25&gt;0, F25&gt;0), "Q1", IF(AND($B25&lt;0, F25&gt;0), "Q2", IF(AND($B25&lt;0, F25&lt;0), "Q3", "Q4")))</f>
+      <c r="L25" s="28" t="str">
+        <f t="shared" si="13"/>
         <v>Q2</v>
       </c>
-      <c r="M25" s="29" t="str">
-        <f>IF(AND($B25&gt;0, G25&gt;0), "Q1", IF(AND($B25&lt;0, G25&gt;0), "Q2", IF(AND($B25&lt;0, G25&lt;0), "Q3", "Q4")))</f>
+      <c r="M25" s="28" t="str">
+        <f t="shared" si="13"/>
         <v>Q2</v>
       </c>
-      <c r="O25" s="29" t="str">
-        <f t="shared" si="9"/>
-        <v>Correct</v>
-      </c>
-      <c r="P25" s="34" t="str">
-        <f t="shared" si="10"/>
+      <c r="O25" s="28" t="str">
+        <f t="shared" si="15"/>
+        <v>Correct</v>
+      </c>
+      <c r="P25" s="31" t="str">
+        <f t="shared" si="16"/>
         <v>Incorrect</v>
       </c>
-      <c r="Q25" s="29" t="str">
-        <f t="shared" si="11"/>
-        <v>Correct</v>
-      </c>
-      <c r="R25" s="29" t="str">
-        <f t="shared" si="12"/>
-        <v>Correct</v>
-      </c>
-      <c r="S25" s="29" t="str">
+      <c r="Q25" s="28" t="str">
+        <f t="shared" si="17"/>
+        <v>Correct</v>
+      </c>
+      <c r="R25" s="28" t="str">
+        <f t="shared" si="18"/>
+        <v>Correct</v>
+      </c>
+      <c r="S25" s="28" t="str">
         <f>IF(OR(M25="Q2", M25="Q4"), "Correct", "Incorrect")</f>
         <v>Correct</v>
       </c>

</xml_diff>